<commit_message>
Add boolean support in ExcelDb using boolean_keys parameter
</commit_message>
<xml_diff>
--- a/inventory/db/template.xlsx
+++ b/inventory/db/template.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,52 +442,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>a1</t>
+          <t>my a</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>a2</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>a3</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>my a</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C5" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>